<commit_message>
Final - 23 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757CD6F8-C570-467F-9195-2A0C24377785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570048A-6399-4AC6-A5A2-6DC349E0A0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Subject</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Warning Msg</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
     <t>Reason</t>
   </si>
   <si>
@@ -316,15 +313,9 @@
     <t>Comment2</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
     <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm.</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
     <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm</t>
   </si>
   <si>
@@ -332,6 +323,9 @@
   </si>
   <si>
     <t>Sellside</t>
+  </si>
+  <si>
+    <t>Companies closed with is missing. Please add a counterparty and a closing bid.</t>
   </si>
 </sst>
 </file>
@@ -697,7 +691,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -705,7 +699,7 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -826,14 +820,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.88671875" customWidth="1"/>
-    <col min="2" max="3" width="66.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -841,22 +836,18 @@
         <v>79</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -867,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -976,13 +967,13 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1230,30 +1221,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round Trip - Sellside - Add Counterparty
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570048A-6399-4AC6-A5A2-6DC349E0A0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15478F85-06EF-4CD0-A0DE-A2017AA19B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="AddOpportunity" sheetId="12" r:id="rId6"/>
     <sheet name="CompanyUpdates" sheetId="16" r:id="rId7"/>
     <sheet name="AddContact" sheetId="13" r:id="rId8"/>
-    <sheet name="FlagReason" sheetId="18" r:id="rId9"/>
+    <sheet name="AddCounterparty" sheetId="19" r:id="rId9"/>
+    <sheet name="FlagReason" sheetId="18" r:id="rId10"/>
+    <sheet name="Bid" sheetId="20" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
   <si>
     <t>Subject</t>
   </si>
@@ -326,6 +328,27 @@
   </si>
   <si>
     <t>Companies closed with is missing. Please add a counterparty and a closing bid.</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Round Name</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -708,6 +731,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="4" width="44.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1801C156-FF51-48D1-AFDE-99F0B5B804EF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5A9CA0-9D6D-4A18-8830-C9EDB8538004}">
   <dimension ref="A1:A4"/>
@@ -820,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -858,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,46 +1310,33 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BE388F-08B7-42DA-B23E-9E2AE4994E43}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="3" max="4" width="44.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>90</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip - Initial - 2nd July 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15478F85-06EF-4CD0-A0DE-A2017AA19B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA7CC9D-17AA-4C24-AFEC-650AB532DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t>Subject</t>
   </si>
@@ -315,12 +315,6 @@
     <t>Comment2</t>
   </si>
   <si>
-    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm.</t>
-  </si>
-  <si>
-    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm</t>
-  </si>
-  <si>
     <t>Zillow Home Loans, LLC</t>
   </si>
   <si>
@@ -349,6 +343,12 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Triangle Capital Corporation</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,19 +760,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -783,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1801C156-FF51-48D1-AFDE-99F0B5B804EF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -794,18 +790,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +922,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,11 +943,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="C2" s="7"/>
     </row>
   </sheetData>
@@ -961,15 +959,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
@@ -1072,13 +1070,13 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1159,6 +1157,98 @@
         <v>65</v>
       </c>
       <c r="AD2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1311,32 +1401,40 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BE388F-08B7-42DA-B23E-9E2AE4994E43}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round Trip - Sellside - Subject - Final - 2nd July 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_SubjectIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA7CC9D-17AA-4C24-AFEC-650AB532DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B52610E-9B81-4E18-B634-2C918912A53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="112">
   <si>
     <t>Subject</t>
   </si>
@@ -349,13 +349,46 @@
   </si>
   <si>
     <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Assured Guaranty Ltd.</t>
+  </si>
+  <si>
+    <t>Comment3</t>
+  </si>
+  <si>
+    <t>Minnesota Rubber &amp; Plastics</t>
+  </si>
+  <si>
+    <t>Trelleborg AB</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm.</t>
+  </si>
+  <si>
+    <t>Warning Msg 4</t>
+  </si>
+  <si>
+    <t>ShowingTime</t>
+  </si>
+  <si>
+    <t>Zillow, Inc.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to either capital provider or operating company that is Private Equity owned. Please reach out to Brian Miller to help confirm</t>
+  </si>
+  <si>
+    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as a Private Equity/Hedge Fund/Family Office company or an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Subject a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +400,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,18 +796,22 @@
         <v>88</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -919,7 +962,57 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
+  <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -927,48 +1020,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:AD3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -1252,6 +1304,190 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" t="s">
+        <v>73</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1262,7 +1498,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BE388F-08B7-42DA-B23E-9E2AE4994E43}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,9 +1667,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>